<commit_message>
Updates to file structures from R
</commit_message>
<xml_diff>
--- a/Census/US Census, Population By State, 2020-2022.xlsx
+++ b/Census/US Census, Population By State, 2020-2022.xlsx
@@ -8,24 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joesimeone/Desktop/R Master/DPC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BCCF96CC-8A9B-5D4E-84DC-4DFF613836E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5DAD699-24FB-F34F-B546-5C5644C638FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16080" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16340" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NST-EST2022-POP" sheetId="1" r:id="rId1"/>
+    <sheet name="EST 2022 POP" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_NST01">'NST-EST2022-POP'!$A$4:$E$62</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'NST-EST2022-POP'!$A$2:$E$67</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">'NST-EST2022-POP'!$A:$A,'NST-EST2022-POP'!$2:$4</definedName>
+    <definedName name="_NST01">'NST-EST2022-POP'!$A$2:$E$60</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'NST-EST2022-POP'!$A$2:$E$65</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">'NST-EST2022-POP'!$A:$A,'NST-EST2022-POP'!$2:$2</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="65">
   <si>
     <t>United States</t>
   </si>
@@ -45,16 +46,10 @@
     <t>table with row headers in column A and column headers in rows 3 through 4. (leading dots indicate sub-parts)</t>
   </si>
   <si>
-    <t>Annual Estimates of the Resident Population for the United States, Regions, States, District of Columbia, and Puerto Rico: April 1, 2020 to July 1, 2022</t>
-  </si>
-  <si>
     <t>Geographic Area</t>
   </si>
   <si>
     <t>April 1, 2020 Estimates Base</t>
-  </si>
-  <si>
-    <t>Population Estimate (as of July 1)</t>
   </si>
   <si>
     <r>
@@ -1010,7 +1005,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -1053,10 +1048,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -1065,6 +1056,10 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
@@ -1087,34 +1082,6 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
@@ -1124,6 +1091,21 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1464,10 +1446,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:E67"/>
+  <dimension ref="A1:E65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
@@ -1486,124 +1468,140 @@
       <c r="D1" s="25"/>
       <c r="E1" s="25"/>
     </row>
-    <row r="2" spans="1:5" ht="28.5" customHeight="1">
-      <c r="A2" s="26" t="s">
+    <row r="2" spans="1:5" s="2" customFormat="1" ht="24.75" customHeight="1">
+      <c r="A2" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-    </row>
-    <row r="3" spans="1:5" s="12" customFormat="1" ht="24.75" customHeight="1">
-      <c r="A3" s="28" t="s">
+      <c r="B2" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-    </row>
-    <row r="4" spans="1:5" s="2" customFormat="1" ht="24.75" customHeight="1">
-      <c r="A4" s="29"/>
-      <c r="B4" s="29"/>
-      <c r="C4" s="3">
+      <c r="C2" s="3">
         <v>2020</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D2" s="3">
         <v>2021</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E2" s="3">
         <v>2022</v>
       </c>
     </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="5">
+        <v>331449520</v>
+      </c>
+      <c r="C3" s="5">
+        <v>331511512</v>
+      </c>
+      <c r="D3" s="5">
+        <v>332031554</v>
+      </c>
+      <c r="E3" s="5">
+        <v>333287557</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="7">
+        <v>57609156</v>
+      </c>
+      <c r="C4" s="7">
+        <v>57448898</v>
+      </c>
+      <c r="D4" s="7">
+        <v>57259257</v>
+      </c>
+      <c r="E4" s="7">
+        <v>57040406</v>
+      </c>
+    </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="5">
-        <v>331449520</v>
-      </c>
-      <c r="C5" s="5">
-        <v>331511512</v>
-      </c>
-      <c r="D5" s="5">
-        <v>332031554</v>
-      </c>
-      <c r="E5" s="5">
-        <v>333287557</v>
+      <c r="A5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="7">
+        <v>68985537</v>
+      </c>
+      <c r="C5" s="7">
+        <v>68961043</v>
+      </c>
+      <c r="D5" s="7">
+        <v>68836505</v>
+      </c>
+      <c r="E5" s="7">
+        <v>68787595</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="6" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B6" s="7">
-        <v>57609156</v>
+        <v>126266262</v>
       </c>
       <c r="C6" s="7">
-        <v>57448898</v>
+        <v>126450613</v>
       </c>
       <c r="D6" s="7">
-        <v>57259257</v>
+        <v>127346029</v>
       </c>
       <c r="E6" s="7">
-        <v>57040406</v>
+        <v>128716192</v>
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="7">
-        <v>68985537</v>
-      </c>
-      <c r="C7" s="7">
-        <v>68961043</v>
-      </c>
-      <c r="D7" s="7">
-        <v>68836505</v>
-      </c>
-      <c r="E7" s="7">
-        <v>68787595</v>
+      <c r="A7" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="9">
+        <v>78588565</v>
+      </c>
+      <c r="C7" s="9">
+        <v>78650958</v>
+      </c>
+      <c r="D7" s="9">
+        <v>78589763</v>
+      </c>
+      <c r="E7" s="9">
+        <v>78743364</v>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="6" t="s">
-        <v>3</v>
+      <c r="A8" s="10" t="s">
+        <v>8</v>
       </c>
       <c r="B8" s="7">
-        <v>126266262</v>
+        <v>5024356</v>
       </c>
       <c r="C8" s="7">
-        <v>126450613</v>
+        <v>5031362</v>
       </c>
       <c r="D8" s="7">
-        <v>127346029</v>
+        <v>5049846</v>
       </c>
       <c r="E8" s="7">
-        <v>128716192</v>
+        <v>5074296</v>
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="9">
-        <v>78588565</v>
-      </c>
-      <c r="C9" s="9">
-        <v>78650958</v>
-      </c>
-      <c r="D9" s="9">
-        <v>78589763</v>
-      </c>
-      <c r="E9" s="9">
-        <v>78743364</v>
+      <c r="A9" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="7">
+        <v>733378</v>
+      </c>
+      <c r="C9" s="7">
+        <v>732923</v>
+      </c>
+      <c r="D9" s="7">
+        <v>734182</v>
+      </c>
+      <c r="E9" s="7">
+        <v>733583</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1611,16 +1609,16 @@
         <v>10</v>
       </c>
       <c r="B10" s="7">
-        <v>5024356</v>
+        <v>7151507</v>
       </c>
       <c r="C10" s="7">
-        <v>5031362</v>
+        <v>7179943</v>
       </c>
       <c r="D10" s="7">
-        <v>5049846</v>
+        <v>7264877</v>
       </c>
       <c r="E10" s="7">
-        <v>5074296</v>
+        <v>7359197</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1628,16 +1626,16 @@
         <v>11</v>
       </c>
       <c r="B11" s="7">
-        <v>733378</v>
+        <v>3011555</v>
       </c>
       <c r="C11" s="7">
-        <v>732923</v>
+        <v>3014195</v>
       </c>
       <c r="D11" s="7">
-        <v>734182</v>
+        <v>3028122</v>
       </c>
       <c r="E11" s="7">
-        <v>733583</v>
+        <v>3045637</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1645,16 +1643,16 @@
         <v>12</v>
       </c>
       <c r="B12" s="7">
-        <v>7151507</v>
+        <v>39538245</v>
       </c>
       <c r="C12" s="7">
-        <v>7179943</v>
+        <v>39501653</v>
       </c>
       <c r="D12" s="7">
-        <v>7264877</v>
+        <v>39142991</v>
       </c>
       <c r="E12" s="7">
-        <v>7359197</v>
+        <v>39029342</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1662,16 +1660,16 @@
         <v>13</v>
       </c>
       <c r="B13" s="7">
-        <v>3011555</v>
+        <v>5773733</v>
       </c>
       <c r="C13" s="7">
-        <v>3014195</v>
+        <v>5784865</v>
       </c>
       <c r="D13" s="7">
-        <v>3028122</v>
+        <v>5811297</v>
       </c>
       <c r="E13" s="7">
-        <v>3045637</v>
+        <v>5839926</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1679,16 +1677,16 @@
         <v>14</v>
       </c>
       <c r="B14" s="7">
-        <v>39538245</v>
+        <v>3605942</v>
       </c>
       <c r="C14" s="7">
-        <v>39501653</v>
+        <v>3597362</v>
       </c>
       <c r="D14" s="7">
-        <v>39142991</v>
+        <v>3623355</v>
       </c>
       <c r="E14" s="7">
-        <v>39029342</v>
+        <v>3626205</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1696,16 +1694,16 @@
         <v>15</v>
       </c>
       <c r="B15" s="7">
-        <v>5773733</v>
+        <v>989957</v>
       </c>
       <c r="C15" s="7">
-        <v>5784865</v>
+        <v>992114</v>
       </c>
       <c r="D15" s="7">
-        <v>5811297</v>
+        <v>1004807</v>
       </c>
       <c r="E15" s="7">
-        <v>5839926</v>
+        <v>1018396</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -1713,16 +1711,16 @@
         <v>16</v>
       </c>
       <c r="B16" s="7">
-        <v>3605942</v>
+        <v>689546</v>
       </c>
       <c r="C16" s="7">
-        <v>3597362</v>
+        <v>670868</v>
       </c>
       <c r="D16" s="7">
-        <v>3623355</v>
+        <v>668791</v>
       </c>
       <c r="E16" s="7">
-        <v>3626205</v>
+        <v>671803</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1730,16 +1728,16 @@
         <v>17</v>
       </c>
       <c r="B17" s="7">
-        <v>989957</v>
+        <v>21538226</v>
       </c>
       <c r="C17" s="7">
-        <v>992114</v>
+        <v>21589602</v>
       </c>
       <c r="D17" s="7">
-        <v>1004807</v>
+        <v>21828069</v>
       </c>
       <c r="E17" s="7">
-        <v>1018396</v>
+        <v>22244823</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -1747,16 +1745,16 @@
         <v>18</v>
       </c>
       <c r="B18" s="7">
-        <v>689546</v>
+        <v>10711937</v>
       </c>
       <c r="C18" s="7">
-        <v>670868</v>
+        <v>10729828</v>
       </c>
       <c r="D18" s="7">
-        <v>668791</v>
+        <v>10788029</v>
       </c>
       <c r="E18" s="7">
-        <v>671803</v>
+        <v>10912876</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1764,16 +1762,16 @@
         <v>19</v>
       </c>
       <c r="B19" s="7">
-        <v>21538226</v>
+        <v>1455273</v>
       </c>
       <c r="C19" s="7">
-        <v>21589602</v>
+        <v>1451043</v>
       </c>
       <c r="D19" s="7">
-        <v>21828069</v>
+        <v>1447154</v>
       </c>
       <c r="E19" s="7">
-        <v>22244823</v>
+        <v>1440196</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1781,16 +1779,16 @@
         <v>20</v>
       </c>
       <c r="B20" s="7">
-        <v>10711937</v>
+        <v>1839092</v>
       </c>
       <c r="C20" s="7">
-        <v>10729828</v>
+        <v>1849202</v>
       </c>
       <c r="D20" s="7">
-        <v>10788029</v>
+        <v>1904314</v>
       </c>
       <c r="E20" s="7">
-        <v>10912876</v>
+        <v>1939033</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -1798,16 +1796,16 @@
         <v>21</v>
       </c>
       <c r="B21" s="7">
-        <v>1455273</v>
+        <v>12812545</v>
       </c>
       <c r="C21" s="7">
-        <v>1451043</v>
+        <v>12786580</v>
       </c>
       <c r="D21" s="7">
-        <v>1447154</v>
+        <v>12686469</v>
       </c>
       <c r="E21" s="7">
-        <v>1440196</v>
+        <v>12582032</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -1815,16 +1813,16 @@
         <v>22</v>
       </c>
       <c r="B22" s="7">
-        <v>1839092</v>
+        <v>6785668</v>
       </c>
       <c r="C22" s="7">
-        <v>1849202</v>
+        <v>6788799</v>
       </c>
       <c r="D22" s="7">
-        <v>1904314</v>
+        <v>6813532</v>
       </c>
       <c r="E22" s="7">
-        <v>1939033</v>
+        <v>6833037</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -1832,16 +1830,16 @@
         <v>23</v>
       </c>
       <c r="B23" s="7">
-        <v>12812545</v>
+        <v>3190372</v>
       </c>
       <c r="C23" s="7">
-        <v>12786580</v>
+        <v>3190571</v>
       </c>
       <c r="D23" s="7">
-        <v>12686469</v>
+        <v>3197689</v>
       </c>
       <c r="E23" s="7">
-        <v>12582032</v>
+        <v>3200517</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1849,16 +1847,16 @@
         <v>24</v>
       </c>
       <c r="B24" s="7">
-        <v>6785668</v>
+        <v>2937847</v>
       </c>
       <c r="C24" s="7">
-        <v>6788799</v>
+        <v>2937919</v>
       </c>
       <c r="D24" s="7">
-        <v>6813532</v>
+        <v>2937922</v>
       </c>
       <c r="E24" s="7">
-        <v>6833037</v>
+        <v>2937150</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -1866,16 +1864,16 @@
         <v>25</v>
       </c>
       <c r="B25" s="7">
-        <v>3190372</v>
+        <v>4505893</v>
       </c>
       <c r="C25" s="7">
-        <v>3190571</v>
+        <v>4507445</v>
       </c>
       <c r="D25" s="7">
-        <v>3197689</v>
+        <v>4506589</v>
       </c>
       <c r="E25" s="7">
-        <v>3200517</v>
+        <v>4512310</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -1883,16 +1881,16 @@
         <v>26</v>
       </c>
       <c r="B26" s="7">
-        <v>2937847</v>
+        <v>4657749</v>
       </c>
       <c r="C26" s="7">
-        <v>2937919</v>
+        <v>4651664</v>
       </c>
       <c r="D26" s="7">
-        <v>2937922</v>
+        <v>4627098</v>
       </c>
       <c r="E26" s="7">
-        <v>2937150</v>
+        <v>4590241</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -1900,16 +1898,16 @@
         <v>27</v>
       </c>
       <c r="B27" s="7">
-        <v>4505893</v>
+        <v>1362341</v>
       </c>
       <c r="C27" s="7">
-        <v>4507445</v>
+        <v>1363557</v>
       </c>
       <c r="D27" s="7">
-        <v>4506589</v>
+        <v>1377238</v>
       </c>
       <c r="E27" s="7">
-        <v>4512310</v>
+        <v>1385340</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -1917,16 +1915,16 @@
         <v>28</v>
       </c>
       <c r="B28" s="7">
-        <v>4657749</v>
+        <v>6177213</v>
       </c>
       <c r="C28" s="7">
-        <v>4651664</v>
+        <v>6173205</v>
       </c>
       <c r="D28" s="7">
-        <v>4627098</v>
+        <v>6174610</v>
       </c>
       <c r="E28" s="7">
-        <v>4590241</v>
+        <v>6164660</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -1934,16 +1932,16 @@
         <v>29</v>
       </c>
       <c r="B29" s="7">
-        <v>1362341</v>
+        <v>7029949</v>
       </c>
       <c r="C29" s="7">
-        <v>1363557</v>
+        <v>6995729</v>
       </c>
       <c r="D29" s="7">
-        <v>1377238</v>
+        <v>6989690</v>
       </c>
       <c r="E29" s="7">
-        <v>1385340</v>
+        <v>6981974</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -1951,16 +1949,16 @@
         <v>30</v>
       </c>
       <c r="B30" s="7">
-        <v>6177213</v>
+        <v>10077325</v>
       </c>
       <c r="C30" s="7">
-        <v>6173205</v>
+        <v>10069577</v>
       </c>
       <c r="D30" s="7">
-        <v>6174610</v>
+        <v>10037504</v>
       </c>
       <c r="E30" s="7">
-        <v>6164660</v>
+        <v>10034113</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -1968,16 +1966,16 @@
         <v>31</v>
       </c>
       <c r="B31" s="7">
-        <v>7029949</v>
+        <v>5706504</v>
       </c>
       <c r="C31" s="7">
-        <v>6995729</v>
+        <v>5709852</v>
       </c>
       <c r="D31" s="7">
-        <v>6989690</v>
+        <v>5711471</v>
       </c>
       <c r="E31" s="7">
-        <v>6981974</v>
+        <v>5717184</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -1985,16 +1983,16 @@
         <v>32</v>
       </c>
       <c r="B32" s="7">
-        <v>10077325</v>
+        <v>2961288</v>
       </c>
       <c r="C32" s="7">
-        <v>10069577</v>
+        <v>2958141</v>
       </c>
       <c r="D32" s="7">
-        <v>10037504</v>
+        <v>2949586</v>
       </c>
       <c r="E32" s="7">
-        <v>10034113</v>
+        <v>2940057</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -2002,16 +2000,16 @@
         <v>33</v>
       </c>
       <c r="B33" s="7">
-        <v>5706504</v>
+        <v>6154920</v>
       </c>
       <c r="C33" s="7">
-        <v>5709852</v>
+        <v>6153998</v>
       </c>
       <c r="D33" s="7">
-        <v>5711471</v>
+        <v>6169823</v>
       </c>
       <c r="E33" s="7">
-        <v>5717184</v>
+        <v>6177957</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -2019,16 +2017,16 @@
         <v>34</v>
       </c>
       <c r="B34" s="7">
-        <v>2961288</v>
+        <v>1084197</v>
       </c>
       <c r="C34" s="7">
-        <v>2958141</v>
+        <v>1087075</v>
       </c>
       <c r="D34" s="7">
-        <v>2949586</v>
+        <v>1106227</v>
       </c>
       <c r="E34" s="7">
-        <v>2940057</v>
+        <v>1122867</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -2036,16 +2034,16 @@
         <v>35</v>
       </c>
       <c r="B35" s="7">
-        <v>6154920</v>
+        <v>1961489</v>
       </c>
       <c r="C35" s="7">
-        <v>6153998</v>
+        <v>1962642</v>
       </c>
       <c r="D35" s="7">
-        <v>6169823</v>
+        <v>1963554</v>
       </c>
       <c r="E35" s="7">
-        <v>6177957</v>
+        <v>1967923</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -2053,16 +2051,16 @@
         <v>36</v>
       </c>
       <c r="B36" s="7">
-        <v>1084197</v>
+        <v>3104624</v>
       </c>
       <c r="C36" s="7">
-        <v>1087075</v>
+        <v>3115648</v>
       </c>
       <c r="D36" s="7">
-        <v>1106227</v>
+        <v>3146402</v>
       </c>
       <c r="E36" s="7">
-        <v>1122867</v>
+        <v>3177772</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -2070,16 +2068,16 @@
         <v>37</v>
       </c>
       <c r="B37" s="7">
-        <v>1961489</v>
+        <v>1377518</v>
       </c>
       <c r="C37" s="7">
-        <v>1962642</v>
+        <v>1378587</v>
       </c>
       <c r="D37" s="7">
-        <v>1963554</v>
+        <v>1387505</v>
       </c>
       <c r="E37" s="7">
-        <v>1967923</v>
+        <v>1395231</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -2087,16 +2085,16 @@
         <v>38</v>
       </c>
       <c r="B38" s="7">
-        <v>3104624</v>
+        <v>9289031</v>
       </c>
       <c r="C38" s="7">
-        <v>3115648</v>
+        <v>9271689</v>
       </c>
       <c r="D38" s="7">
-        <v>3146402</v>
+        <v>9267961</v>
       </c>
       <c r="E38" s="7">
-        <v>3177772</v>
+        <v>9261699</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -2104,16 +2102,16 @@
         <v>39</v>
       </c>
       <c r="B39" s="7">
-        <v>1377518</v>
+        <v>2117527</v>
       </c>
       <c r="C39" s="7">
-        <v>1378587</v>
+        <v>2118390</v>
       </c>
       <c r="D39" s="7">
-        <v>1387505</v>
+        <v>2116677</v>
       </c>
       <c r="E39" s="7">
-        <v>1395231</v>
+        <v>2113344</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -2121,16 +2119,16 @@
         <v>40</v>
       </c>
       <c r="B40" s="7">
-        <v>9289031</v>
+        <v>20201230</v>
       </c>
       <c r="C40" s="7">
-        <v>9271689</v>
+        <v>20108296</v>
       </c>
       <c r="D40" s="7">
-        <v>9267961</v>
+        <v>19857492</v>
       </c>
       <c r="E40" s="7">
-        <v>9261699</v>
+        <v>19677151</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -2138,16 +2136,16 @@
         <v>41</v>
       </c>
       <c r="B41" s="7">
-        <v>2117527</v>
+        <v>10439414</v>
       </c>
       <c r="C41" s="7">
-        <v>2118390</v>
+        <v>10449445</v>
       </c>
       <c r="D41" s="7">
-        <v>2116677</v>
+        <v>10565885</v>
       </c>
       <c r="E41" s="7">
-        <v>2113344</v>
+        <v>10698973</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -2155,16 +2153,16 @@
         <v>42</v>
       </c>
       <c r="B42" s="7">
-        <v>20201230</v>
+        <v>779091</v>
       </c>
       <c r="C42" s="7">
-        <v>20108296</v>
+        <v>779518</v>
       </c>
       <c r="D42" s="7">
-        <v>19857492</v>
+        <v>777934</v>
       </c>
       <c r="E42" s="7">
-        <v>19677151</v>
+        <v>779261</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -2172,16 +2170,16 @@
         <v>43</v>
       </c>
       <c r="B43" s="7">
-        <v>10439414</v>
+        <v>11799374</v>
       </c>
       <c r="C43" s="7">
-        <v>10449445</v>
+        <v>11797517</v>
       </c>
       <c r="D43" s="7">
-        <v>10565885</v>
+        <v>11764342</v>
       </c>
       <c r="E43" s="7">
-        <v>10698973</v>
+        <v>11756058</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -2189,16 +2187,16 @@
         <v>44</v>
       </c>
       <c r="B44" s="7">
-        <v>779091</v>
+        <v>3959346</v>
       </c>
       <c r="C44" s="7">
-        <v>779518</v>
+        <v>3964912</v>
       </c>
       <c r="D44" s="7">
-        <v>777934</v>
+        <v>3991225</v>
       </c>
       <c r="E44" s="7">
-        <v>779261</v>
+        <v>4019800</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -2206,16 +2204,16 @@
         <v>45</v>
       </c>
       <c r="B45" s="7">
-        <v>11799374</v>
+        <v>4237291</v>
       </c>
       <c r="C45" s="7">
-        <v>11797517</v>
+        <v>4244795</v>
       </c>
       <c r="D45" s="7">
-        <v>11764342</v>
+        <v>4256301</v>
       </c>
       <c r="E45" s="7">
-        <v>11756058</v>
+        <v>4240137</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -2223,16 +2221,16 @@
         <v>46</v>
       </c>
       <c r="B46" s="7">
-        <v>3959346</v>
+        <v>13002689</v>
       </c>
       <c r="C46" s="7">
-        <v>3964912</v>
+        <v>12994440</v>
       </c>
       <c r="D46" s="7">
-        <v>3991225</v>
+        <v>13012059</v>
       </c>
       <c r="E46" s="7">
-        <v>4019800</v>
+        <v>12972008</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -2240,16 +2238,16 @@
         <v>47</v>
       </c>
       <c r="B47" s="7">
-        <v>4237291</v>
+        <v>1097371</v>
       </c>
       <c r="C47" s="7">
-        <v>4244795</v>
+        <v>1096345</v>
       </c>
       <c r="D47" s="7">
-        <v>4256301</v>
+        <v>1096985</v>
       </c>
       <c r="E47" s="7">
-        <v>4240137</v>
+        <v>1093734</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -2257,16 +2255,16 @@
         <v>48</v>
       </c>
       <c r="B48" s="7">
-        <v>13002689</v>
+        <v>5118429</v>
       </c>
       <c r="C48" s="7">
-        <v>12994440</v>
+        <v>5131848</v>
       </c>
       <c r="D48" s="7">
-        <v>13012059</v>
+        <v>5193266</v>
       </c>
       <c r="E48" s="7">
-        <v>12972008</v>
+        <v>5282634</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -2274,16 +2272,16 @@
         <v>49</v>
       </c>
       <c r="B49" s="7">
-        <v>1097371</v>
+        <v>886677</v>
       </c>
       <c r="C49" s="7">
-        <v>1096345</v>
+        <v>887799</v>
       </c>
       <c r="D49" s="7">
-        <v>1096985</v>
+        <v>896164</v>
       </c>
       <c r="E49" s="7">
-        <v>1093734</v>
+        <v>909824</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -2291,16 +2289,16 @@
         <v>50</v>
       </c>
       <c r="B50" s="7">
-        <v>5118429</v>
+        <v>6910786</v>
       </c>
       <c r="C50" s="7">
-        <v>5131848</v>
+        <v>6925619</v>
       </c>
       <c r="D50" s="7">
-        <v>5193266</v>
+        <v>6968351</v>
       </c>
       <c r="E50" s="7">
-        <v>5282634</v>
+        <v>7051339</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -2308,16 +2306,16 @@
         <v>51</v>
       </c>
       <c r="B51" s="7">
-        <v>886677</v>
+        <v>29145428</v>
       </c>
       <c r="C51" s="7">
-        <v>887799</v>
+        <v>29232474</v>
       </c>
       <c r="D51" s="7">
-        <v>896164</v>
+        <v>29558864</v>
       </c>
       <c r="E51" s="7">
-        <v>909824</v>
+        <v>30029572</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -2325,16 +2323,16 @@
         <v>52</v>
       </c>
       <c r="B52" s="7">
-        <v>6910786</v>
+        <v>3271614</v>
       </c>
       <c r="C52" s="7">
-        <v>6925619</v>
+        <v>3283785</v>
       </c>
       <c r="D52" s="7">
-        <v>6968351</v>
+        <v>3339113</v>
       </c>
       <c r="E52" s="7">
-        <v>7051339</v>
+        <v>3380800</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -2342,16 +2340,16 @@
         <v>53</v>
       </c>
       <c r="B53" s="7">
-        <v>29145428</v>
+        <v>643085</v>
       </c>
       <c r="C53" s="7">
-        <v>29232474</v>
+        <v>642893</v>
       </c>
       <c r="D53" s="7">
-        <v>29558864</v>
+        <v>646972</v>
       </c>
       <c r="E53" s="7">
-        <v>30029572</v>
+        <v>647064</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -2359,16 +2357,16 @@
         <v>54</v>
       </c>
       <c r="B54" s="7">
-        <v>3271614</v>
+        <v>8631384</v>
       </c>
       <c r="C54" s="7">
-        <v>3283785</v>
+        <v>8636471</v>
       </c>
       <c r="D54" s="7">
-        <v>3339113</v>
+        <v>8657365</v>
       </c>
       <c r="E54" s="7">
-        <v>3380800</v>
+        <v>8683619</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -2376,16 +2374,16 @@
         <v>55</v>
       </c>
       <c r="B55" s="7">
-        <v>643085</v>
+        <v>7705247</v>
       </c>
       <c r="C55" s="7">
-        <v>642893</v>
+        <v>7724031</v>
       </c>
       <c r="D55" s="7">
-        <v>646972</v>
+        <v>7740745</v>
       </c>
       <c r="E55" s="7">
-        <v>647064</v>
+        <v>7785786</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -2393,16 +2391,16 @@
         <v>56</v>
       </c>
       <c r="B56" s="7">
-        <v>8631384</v>
+        <v>1793755</v>
       </c>
       <c r="C56" s="7">
-        <v>8636471</v>
+        <v>1791420</v>
       </c>
       <c r="D56" s="7">
-        <v>8657365</v>
+        <v>1785526</v>
       </c>
       <c r="E56" s="7">
-        <v>8683619</v>
+        <v>1775156</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -2410,16 +2408,16 @@
         <v>57</v>
       </c>
       <c r="B57" s="7">
-        <v>7705247</v>
+        <v>5893725</v>
       </c>
       <c r="C57" s="7">
-        <v>7724031</v>
+        <v>5896271</v>
       </c>
       <c r="D57" s="7">
-        <v>7740745</v>
+        <v>5880101</v>
       </c>
       <c r="E57" s="7">
-        <v>7785786</v>
+        <v>5892539</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -2427,133 +2425,95 @@
         <v>58</v>
       </c>
       <c r="B58" s="7">
-        <v>1793755</v>
+        <v>576837</v>
       </c>
       <c r="C58" s="7">
-        <v>1791420</v>
+        <v>577605</v>
       </c>
       <c r="D58" s="7">
-        <v>1785526</v>
+        <v>579483</v>
       </c>
       <c r="E58" s="7">
-        <v>1775156</v>
+        <v>581381</v>
       </c>
     </row>
     <row r="59" spans="1:5">
-      <c r="A59" s="10" t="s">
+      <c r="A59" s="11"/>
+      <c r="B59" s="7"/>
+      <c r="C59" s="7"/>
+      <c r="D59" s="7"/>
+      <c r="E59" s="7"/>
+    </row>
+    <row r="60" spans="1:5" s="14" customFormat="1">
+      <c r="A60" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="B60" s="13">
+        <v>3285874</v>
+      </c>
+      <c r="C60" s="13">
+        <v>3281557</v>
+      </c>
+      <c r="D60" s="13">
+        <v>3262693</v>
+      </c>
+      <c r="E60" s="13">
+        <v>3221789</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="65" customHeight="1">
+      <c r="A61" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="B59" s="7">
-        <v>5893725</v>
-      </c>
-      <c r="C59" s="7">
-        <v>5896271</v>
-      </c>
-      <c r="D59" s="7">
-        <v>5880101</v>
-      </c>
-      <c r="E59" s="7">
-        <v>5892539</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5">
-      <c r="A60" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="B60" s="7">
-        <v>576837</v>
-      </c>
-      <c r="C60" s="7">
-        <v>577605</v>
-      </c>
-      <c r="D60" s="7">
-        <v>579483</v>
-      </c>
-      <c r="E60" s="7">
-        <v>581381</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5">
-      <c r="A61" s="11"/>
-      <c r="B61" s="7"/>
-      <c r="C61" s="7"/>
-      <c r="D61" s="7"/>
-      <c r="E61" s="7"/>
-    </row>
-    <row r="62" spans="1:5" s="15" customFormat="1">
-      <c r="A62" s="13" t="s">
+      <c r="B61" s="27"/>
+      <c r="C61" s="27"/>
+      <c r="D61" s="27"/>
+      <c r="E61" s="28"/>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="B62" s="17"/>
+      <c r="C62" s="17"/>
+      <c r="D62" s="17"/>
+      <c r="E62" s="18"/>
+    </row>
+    <row r="63" spans="1:5" ht="25.5" customHeight="1">
+      <c r="A63" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="B62" s="14">
-        <v>3285874</v>
-      </c>
-      <c r="C62" s="14">
-        <v>3281557</v>
-      </c>
-      <c r="D62" s="14">
-        <v>3262693</v>
-      </c>
-      <c r="E62" s="14">
-        <v>3221789</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" ht="65" customHeight="1">
-      <c r="A63" s="33" t="s">
-        <v>61</v>
-      </c>
-      <c r="B63" s="34"/>
-      <c r="C63" s="34"/>
-      <c r="D63" s="34"/>
-      <c r="E63" s="35"/>
+      <c r="B63" s="20"/>
+      <c r="C63" s="20"/>
+      <c r="D63" s="20"/>
+      <c r="E63" s="21"/>
     </row>
     <row r="64" spans="1:5">
-      <c r="A64" s="16" t="s">
+      <c r="A64" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="B64" s="17"/>
-      <c r="C64" s="17"/>
-      <c r="D64" s="17"/>
-      <c r="E64" s="18"/>
-    </row>
-    <row r="65" spans="1:5" ht="25.5" customHeight="1">
-      <c r="A65" s="19" t="s">
+      <c r="B64" s="20"/>
+      <c r="C64" s="20"/>
+      <c r="D64" s="20"/>
+      <c r="E64" s="21"/>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="B65" s="20"/>
-      <c r="C65" s="20"/>
-      <c r="D65" s="20"/>
-      <c r="E65" s="21"/>
-    </row>
-    <row r="66" spans="1:5">
-      <c r="A66" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="B66" s="20"/>
-      <c r="C66" s="20"/>
-      <c r="D66" s="20"/>
-      <c r="E66" s="21"/>
-    </row>
-    <row r="67" spans="1:5">
-      <c r="A67" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="B67" s="23"/>
-      <c r="C67" s="23"/>
-      <c r="D67" s="23"/>
-      <c r="E67" s="24"/>
+      <c r="B65" s="23"/>
+      <c r="C65" s="23"/>
+      <c r="D65" s="23"/>
+      <c r="E65" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="6">
+    <mergeCell ref="A62:E62"/>
+    <mergeCell ref="A63:E63"/>
     <mergeCell ref="A64:E64"/>
     <mergeCell ref="A65:E65"/>
-    <mergeCell ref="A66:E66"/>
-    <mergeCell ref="A67:E67"/>
     <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="A63:E63"/>
+    <mergeCell ref="A61:E61"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="80" orientation="landscape" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
@@ -2562,4 +2522,988 @@
     <brk id="3" max="1048575" man="1"/>
   </colBreaks>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A48EF5B-1B6A-C244-BFED-0738BD8E7F03}">
+  <dimension ref="A1:E57"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="56">
+      <c r="A1" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D1" s="3">
+        <v>2021</v>
+      </c>
+      <c r="E1" s="3">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="31">
+        <v>331449520</v>
+      </c>
+      <c r="C2" s="31">
+        <v>331511512</v>
+      </c>
+      <c r="D2" s="31">
+        <v>332031554</v>
+      </c>
+      <c r="E2" s="31">
+        <v>333287557</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="31">
+        <v>57609156</v>
+      </c>
+      <c r="C3" s="31">
+        <v>57448898</v>
+      </c>
+      <c r="D3" s="31">
+        <v>57259257</v>
+      </c>
+      <c r="E3" s="31">
+        <v>57040406</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="31">
+        <v>68985537</v>
+      </c>
+      <c r="C4" s="31">
+        <v>68961043</v>
+      </c>
+      <c r="D4" s="31">
+        <v>68836505</v>
+      </c>
+      <c r="E4" s="31">
+        <v>68787595</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="31">
+        <v>126266262</v>
+      </c>
+      <c r="C5" s="31">
+        <v>126450613</v>
+      </c>
+      <c r="D5" s="31">
+        <v>127346029</v>
+      </c>
+      <c r="E5" s="31">
+        <v>128716192</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="31">
+        <v>78588565</v>
+      </c>
+      <c r="C6" s="31">
+        <v>78650958</v>
+      </c>
+      <c r="D6" s="31">
+        <v>78589763</v>
+      </c>
+      <c r="E6" s="31">
+        <v>78743364</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="31">
+        <v>5024356</v>
+      </c>
+      <c r="C7" s="31">
+        <v>5031362</v>
+      </c>
+      <c r="D7" s="31">
+        <v>5049846</v>
+      </c>
+      <c r="E7" s="31">
+        <v>5074296</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="31">
+        <v>733378</v>
+      </c>
+      <c r="C8" s="31">
+        <v>732923</v>
+      </c>
+      <c r="D8" s="31">
+        <v>734182</v>
+      </c>
+      <c r="E8" s="31">
+        <v>733583</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="31">
+        <v>7151507</v>
+      </c>
+      <c r="C9" s="31">
+        <v>7179943</v>
+      </c>
+      <c r="D9" s="31">
+        <v>7264877</v>
+      </c>
+      <c r="E9" s="31">
+        <v>7359197</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="31">
+        <v>3011555</v>
+      </c>
+      <c r="C10" s="31">
+        <v>3014195</v>
+      </c>
+      <c r="D10" s="31">
+        <v>3028122</v>
+      </c>
+      <c r="E10" s="31">
+        <v>3045637</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="31">
+        <v>39538245</v>
+      </c>
+      <c r="C11" s="31">
+        <v>39501653</v>
+      </c>
+      <c r="D11" s="31">
+        <v>39142991</v>
+      </c>
+      <c r="E11" s="31">
+        <v>39029342</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="31">
+        <v>5773733</v>
+      </c>
+      <c r="C12" s="31">
+        <v>5784865</v>
+      </c>
+      <c r="D12" s="31">
+        <v>5811297</v>
+      </c>
+      <c r="E12" s="31">
+        <v>5839926</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="31">
+        <v>3605942</v>
+      </c>
+      <c r="C13" s="31">
+        <v>3597362</v>
+      </c>
+      <c r="D13" s="31">
+        <v>3623355</v>
+      </c>
+      <c r="E13" s="31">
+        <v>3626205</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="31">
+        <v>989957</v>
+      </c>
+      <c r="C14" s="31">
+        <v>992114</v>
+      </c>
+      <c r="D14" s="31">
+        <v>1004807</v>
+      </c>
+      <c r="E14" s="31">
+        <v>1018396</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="31">
+        <v>689546</v>
+      </c>
+      <c r="C15" s="31">
+        <v>670868</v>
+      </c>
+      <c r="D15" s="31">
+        <v>668791</v>
+      </c>
+      <c r="E15" s="31">
+        <v>671803</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="31">
+        <v>21538226</v>
+      </c>
+      <c r="C16" s="31">
+        <v>21589602</v>
+      </c>
+      <c r="D16" s="31">
+        <v>21828069</v>
+      </c>
+      <c r="E16" s="31">
+        <v>22244823</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="31">
+        <v>10711937</v>
+      </c>
+      <c r="C17" s="31">
+        <v>10729828</v>
+      </c>
+      <c r="D17" s="31">
+        <v>10788029</v>
+      </c>
+      <c r="E17" s="31">
+        <v>10912876</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="31">
+        <v>1455273</v>
+      </c>
+      <c r="C18" s="31">
+        <v>1451043</v>
+      </c>
+      <c r="D18" s="31">
+        <v>1447154</v>
+      </c>
+      <c r="E18" s="31">
+        <v>1440196</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="31">
+        <v>1839092</v>
+      </c>
+      <c r="C19" s="31">
+        <v>1849202</v>
+      </c>
+      <c r="D19" s="31">
+        <v>1904314</v>
+      </c>
+      <c r="E19" s="31">
+        <v>1939033</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="31">
+        <v>12812545</v>
+      </c>
+      <c r="C20" s="31">
+        <v>12786580</v>
+      </c>
+      <c r="D20" s="31">
+        <v>12686469</v>
+      </c>
+      <c r="E20" s="31">
+        <v>12582032</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="31">
+        <v>6785668</v>
+      </c>
+      <c r="C21" s="31">
+        <v>6788799</v>
+      </c>
+      <c r="D21" s="31">
+        <v>6813532</v>
+      </c>
+      <c r="E21" s="31">
+        <v>6833037</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="31">
+        <v>3190372</v>
+      </c>
+      <c r="C22" s="31">
+        <v>3190571</v>
+      </c>
+      <c r="D22" s="31">
+        <v>3197689</v>
+      </c>
+      <c r="E22" s="31">
+        <v>3200517</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="31">
+        <v>2937847</v>
+      </c>
+      <c r="C23" s="31">
+        <v>2937919</v>
+      </c>
+      <c r="D23" s="31">
+        <v>2937922</v>
+      </c>
+      <c r="E23" s="31">
+        <v>2937150</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="31">
+        <v>4505893</v>
+      </c>
+      <c r="C24" s="31">
+        <v>4507445</v>
+      </c>
+      <c r="D24" s="31">
+        <v>4506589</v>
+      </c>
+      <c r="E24" s="31">
+        <v>4512310</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="31">
+        <v>4657749</v>
+      </c>
+      <c r="C25" s="31">
+        <v>4651664</v>
+      </c>
+      <c r="D25" s="31">
+        <v>4627098</v>
+      </c>
+      <c r="E25" s="31">
+        <v>4590241</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" s="31">
+        <v>1362341</v>
+      </c>
+      <c r="C26" s="31">
+        <v>1363557</v>
+      </c>
+      <c r="D26" s="31">
+        <v>1377238</v>
+      </c>
+      <c r="E26" s="31">
+        <v>1385340</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" s="31">
+        <v>6177213</v>
+      </c>
+      <c r="C27" s="31">
+        <v>6173205</v>
+      </c>
+      <c r="D27" s="31">
+        <v>6174610</v>
+      </c>
+      <c r="E27" s="31">
+        <v>6164660</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" s="31">
+        <v>7029949</v>
+      </c>
+      <c r="C28" s="31">
+        <v>6995729</v>
+      </c>
+      <c r="D28" s="31">
+        <v>6989690</v>
+      </c>
+      <c r="E28" s="31">
+        <v>6981974</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" s="31">
+        <v>10077325</v>
+      </c>
+      <c r="C29" s="31">
+        <v>10069577</v>
+      </c>
+      <c r="D29" s="31">
+        <v>10037504</v>
+      </c>
+      <c r="E29" s="31">
+        <v>10034113</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" s="31">
+        <v>5706504</v>
+      </c>
+      <c r="C30" s="31">
+        <v>5709852</v>
+      </c>
+      <c r="D30" s="31">
+        <v>5711471</v>
+      </c>
+      <c r="E30" s="31">
+        <v>5717184</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31" s="31">
+        <v>2961288</v>
+      </c>
+      <c r="C31" s="31">
+        <v>2958141</v>
+      </c>
+      <c r="D31" s="31">
+        <v>2949586</v>
+      </c>
+      <c r="E31" s="31">
+        <v>2940057</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32" s="31">
+        <v>6154920</v>
+      </c>
+      <c r="C32" s="31">
+        <v>6153998</v>
+      </c>
+      <c r="D32" s="31">
+        <v>6169823</v>
+      </c>
+      <c r="E32" s="31">
+        <v>6177957</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="B33" s="31">
+        <v>1084197</v>
+      </c>
+      <c r="C33" s="31">
+        <v>1087075</v>
+      </c>
+      <c r="D33" s="31">
+        <v>1106227</v>
+      </c>
+      <c r="E33" s="31">
+        <v>1122867</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34" s="31">
+        <v>1961489</v>
+      </c>
+      <c r="C34" s="31">
+        <v>1962642</v>
+      </c>
+      <c r="D34" s="31">
+        <v>1963554</v>
+      </c>
+      <c r="E34" s="31">
+        <v>1967923</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35" s="31">
+        <v>3104624</v>
+      </c>
+      <c r="C35" s="31">
+        <v>3115648</v>
+      </c>
+      <c r="D35" s="31">
+        <v>3146402</v>
+      </c>
+      <c r="E35" s="31">
+        <v>3177772</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36" s="31">
+        <v>1377518</v>
+      </c>
+      <c r="C36" s="31">
+        <v>1378587</v>
+      </c>
+      <c r="D36" s="31">
+        <v>1387505</v>
+      </c>
+      <c r="E36" s="31">
+        <v>1395231</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37" s="31">
+        <v>9289031</v>
+      </c>
+      <c r="C37" s="31">
+        <v>9271689</v>
+      </c>
+      <c r="D37" s="31">
+        <v>9267961</v>
+      </c>
+      <c r="E37" s="31">
+        <v>9261699</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="B38" s="31">
+        <v>2117527</v>
+      </c>
+      <c r="C38" s="31">
+        <v>2118390</v>
+      </c>
+      <c r="D38" s="31">
+        <v>2116677</v>
+      </c>
+      <c r="E38" s="31">
+        <v>2113344</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="B39" s="31">
+        <v>20201230</v>
+      </c>
+      <c r="C39" s="31">
+        <v>20108296</v>
+      </c>
+      <c r="D39" s="31">
+        <v>19857492</v>
+      </c>
+      <c r="E39" s="31">
+        <v>19677151</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="B40" s="31">
+        <v>10439414</v>
+      </c>
+      <c r="C40" s="31">
+        <v>10449445</v>
+      </c>
+      <c r="D40" s="31">
+        <v>10565885</v>
+      </c>
+      <c r="E40" s="31">
+        <v>10698973</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="B41" s="31">
+        <v>779091</v>
+      </c>
+      <c r="C41" s="31">
+        <v>779518</v>
+      </c>
+      <c r="D41" s="31">
+        <v>777934</v>
+      </c>
+      <c r="E41" s="31">
+        <v>779261</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="B42" s="31">
+        <v>11799374</v>
+      </c>
+      <c r="C42" s="31">
+        <v>11797517</v>
+      </c>
+      <c r="D42" s="31">
+        <v>11764342</v>
+      </c>
+      <c r="E42" s="31">
+        <v>11756058</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="B43" s="31">
+        <v>3959346</v>
+      </c>
+      <c r="C43" s="31">
+        <v>3964912</v>
+      </c>
+      <c r="D43" s="31">
+        <v>3991225</v>
+      </c>
+      <c r="E43" s="31">
+        <v>4019800</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="B44" s="31">
+        <v>4237291</v>
+      </c>
+      <c r="C44" s="31">
+        <v>4244795</v>
+      </c>
+      <c r="D44" s="31">
+        <v>4256301</v>
+      </c>
+      <c r="E44" s="31">
+        <v>4240137</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="B45" s="31">
+        <v>13002689</v>
+      </c>
+      <c r="C45" s="31">
+        <v>12994440</v>
+      </c>
+      <c r="D45" s="31">
+        <v>13012059</v>
+      </c>
+      <c r="E45" s="31">
+        <v>12972008</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="B46" s="31">
+        <v>1097371</v>
+      </c>
+      <c r="C46" s="31">
+        <v>1096345</v>
+      </c>
+      <c r="D46" s="31">
+        <v>1096985</v>
+      </c>
+      <c r="E46" s="31">
+        <v>1093734</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="B47" s="31">
+        <v>5118429</v>
+      </c>
+      <c r="C47" s="31">
+        <v>5131848</v>
+      </c>
+      <c r="D47" s="31">
+        <v>5193266</v>
+      </c>
+      <c r="E47" s="31">
+        <v>5282634</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="B48" s="31">
+        <v>886677</v>
+      </c>
+      <c r="C48" s="31">
+        <v>887799</v>
+      </c>
+      <c r="D48" s="31">
+        <v>896164</v>
+      </c>
+      <c r="E48" s="31">
+        <v>909824</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="B49" s="31">
+        <v>6910786</v>
+      </c>
+      <c r="C49" s="31">
+        <v>6925619</v>
+      </c>
+      <c r="D49" s="31">
+        <v>6968351</v>
+      </c>
+      <c r="E49" s="31">
+        <v>7051339</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="B50" s="31">
+        <v>29145428</v>
+      </c>
+      <c r="C50" s="31">
+        <v>29232474</v>
+      </c>
+      <c r="D50" s="31">
+        <v>29558864</v>
+      </c>
+      <c r="E50" s="31">
+        <v>30029572</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="B51" s="31">
+        <v>3271614</v>
+      </c>
+      <c r="C51" s="31">
+        <v>3283785</v>
+      </c>
+      <c r="D51" s="31">
+        <v>3339113</v>
+      </c>
+      <c r="E51" s="31">
+        <v>3380800</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="B52" s="31">
+        <v>643085</v>
+      </c>
+      <c r="C52" s="31">
+        <v>642893</v>
+      </c>
+      <c r="D52" s="31">
+        <v>646972</v>
+      </c>
+      <c r="E52" s="31">
+        <v>647064</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="B53" s="31">
+        <v>8631384</v>
+      </c>
+      <c r="C53" s="31">
+        <v>8636471</v>
+      </c>
+      <c r="D53" s="31">
+        <v>8657365</v>
+      </c>
+      <c r="E53" s="31">
+        <v>8683619</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="B54" s="31">
+        <v>7705247</v>
+      </c>
+      <c r="C54" s="31">
+        <v>7724031</v>
+      </c>
+      <c r="D54" s="31">
+        <v>7740745</v>
+      </c>
+      <c r="E54" s="31">
+        <v>7785786</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="B55" s="31">
+        <v>1793755</v>
+      </c>
+      <c r="C55" s="31">
+        <v>1791420</v>
+      </c>
+      <c r="D55" s="31">
+        <v>1785526</v>
+      </c>
+      <c r="E55" s="31">
+        <v>1775156</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="B56" s="31">
+        <v>5893725</v>
+      </c>
+      <c r="C56" s="31">
+        <v>5896271</v>
+      </c>
+      <c r="D56" s="31">
+        <v>5880101</v>
+      </c>
+      <c r="E56" s="31">
+        <v>5892539</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="B57" s="31">
+        <v>576837</v>
+      </c>
+      <c r="C57" s="31">
+        <v>577605</v>
+      </c>
+      <c r="D57" s="31">
+        <v>579483</v>
+      </c>
+      <c r="E57" s="31">
+        <v>581381</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>